<commit_message>
added a register of tablewares per table
</commit_message>
<xml_diff>
--- a/TODO vertical slice.xlsx
+++ b/TODO vertical slice.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="24920" windowHeight="10760"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="24915" windowHeight="10755"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -668,17 +668,17 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="78.7265625" customWidth="1"/>
-    <col min="2" max="2" width="12.7265625" customWidth="1"/>
-    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.81640625" customWidth="1"/>
-    <col min="6" max="6" width="31.453125" customWidth="1"/>
+    <col min="1" max="1" width="78.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="31.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -703,22 +703,22 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>46</v>
       </c>
       <c r="C2">
         <v>4</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>51</v>
       </c>
       <c r="F2" t="s">
-        <v>93</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -780,30 +780,30 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6">
         <v>2</v>
       </c>
-      <c r="E6" t="s">
-        <v>29</v>
+      <c r="E6" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="F6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="C7">
         <v>3</v>
@@ -811,19 +811,19 @@
       <c r="D7">
         <v>2</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>51</v>
+      <c r="E7" t="s">
+        <v>29</v>
       </c>
       <c r="F7" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>79</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C8">
         <v>3</v>
@@ -835,15 +835,15 @@
         <v>29</v>
       </c>
       <c r="F8" t="s">
-        <v>43</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -854,33 +854,33 @@
       <c r="E9" t="s">
         <v>29</v>
       </c>
-      <c r="F9" t="s">
-        <v>80</v>
-      </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>74</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>68</v>
+        <v>5</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E10" t="s">
         <v>29</v>
+      </c>
+      <c r="F10" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>92</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -891,93 +891,93 @@
       <c r="E11" t="s">
         <v>29</v>
       </c>
-      <c r="F11" t="s">
-        <v>69</v>
-      </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>92</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" t="s">
         <v>29</v>
+      </c>
+      <c r="F12" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="C13">
         <v>2</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13" t="s">
         <v>29</v>
       </c>
       <c r="F13" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E14" t="s">
         <v>29</v>
       </c>
       <c r="F14" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" t="s">
         <v>29</v>
       </c>
       <c r="F15" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -989,32 +989,32 @@
         <v>29</v>
       </c>
       <c r="F16" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E17" t="s">
         <v>29</v>
       </c>
       <c r="F17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" t="s">
-        <v>71</v>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="30">
+      <c r="A18" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="B18" t="s">
         <v>36</v>
@@ -1029,75 +1029,72 @@
         <v>29</v>
       </c>
       <c r="F18" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="29">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="2" t="s">
-        <v>37</v>
+        <v>76</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>77</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E19" t="s">
         <v>29</v>
       </c>
       <c r="F19" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="2" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E20" t="s">
         <v>29</v>
       </c>
       <c r="F20" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="2" t="s">
-        <v>85</v>
+      <c r="A21" t="s">
+        <v>75</v>
       </c>
       <c r="B21" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="C21">
+        <v>-1</v>
+      </c>
+      <c r="D21">
         <v>0</v>
       </c>
-      <c r="D21">
-        <v>2</v>
-      </c>
-      <c r="E21" t="s">
-        <v>29</v>
-      </c>
-      <c r="F21" t="s">
-        <v>87</v>
+      <c r="E21" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="B22" t="s">
-        <v>65</v>
+        <v>1</v>
       </c>
       <c r="C22">
         <v>-1</v>
@@ -1108,13 +1105,16 @@
       <c r="E22" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="F22" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="B23" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="C23">
         <v>-1</v>
@@ -1125,16 +1125,13 @@
       <c r="E23" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F23" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="C24">
         <v>-1</v>
@@ -1148,7 +1145,7 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="B25" t="s">
         <v>23</v>
@@ -1162,25 +1159,28 @@
       <c r="E25" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="F25" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
       <c r="B26" t="s">
-        <v>23</v>
+        <v>81</v>
       </c>
       <c r="C26">
         <v>-1</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>30</v>
       </c>
       <c r="F26" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1432,10 +1432,10 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:F38">
-    <sortCondition descending="1" ref="C2:C38"/>
-    <sortCondition ref="E2:E38" customList="wip,todo,done"/>
-    <sortCondition ref="D2:D38"/>
+  <sortState ref="A2:F39">
+    <sortCondition descending="1" ref="C2:C39"/>
+    <sortCondition ref="E2:E39" customList="wip,todo,done"/>
+    <sortCondition ref="D2:D39"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1447,7 +1447,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1459,7 +1459,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Ajustement de la position et rotation des couverts au moment de lancer
</commit_message>
<xml_diff>
--- a/TODO vertical slice.xlsx
+++ b/TODO vertical slice.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$F$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$F$34</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="99">
   <si>
     <t>Ajuster inclinaison du target viewer selon la pente de l'objet</t>
   </si>
@@ -307,6 +307,15 @@
   </si>
   <si>
     <t>Pour enrichir le gameplay, dans cette perspective du close world…permettrait de rajouter un peu de variété, et pourquoi pas d'y associer des bonus de points (voire des malus quand on rentre dans un NPC en pleine course)</t>
+  </si>
+  <si>
+    <t>Dans le tableau de scores, remplacer remaining time par missed tables</t>
+  </si>
+  <si>
+    <t>Gérer les collisions du bras et des couverts aux abords d'un mur</t>
+  </si>
+  <si>
+    <t>voir vidéo tuto YouTube</t>
   </si>
 </sst>
 </file>
@@ -671,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -709,7 +718,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -722,9 +731,6 @@
       </c>
       <c r="E2" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="F2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -766,30 +772,30 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>97</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>68</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D5">
         <v>2</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>51</v>
+      <c r="E5" t="s">
+        <v>29</v>
       </c>
       <c r="F5" t="s">
-        <v>61</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -797,19 +803,19 @@
       <c r="D6">
         <v>2</v>
       </c>
-      <c r="E6" t="s">
-        <v>29</v>
+      <c r="E6" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="F6" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7">
         <v>3</v>
@@ -821,15 +827,15 @@
         <v>29</v>
       </c>
       <c r="F7" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="C8">
         <v>3</v>
@@ -840,13 +846,16 @@
       <c r="E8" t="s">
         <v>29</v>
       </c>
+      <c r="F8" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>68</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -857,36 +866,33 @@
       <c r="E9" t="s">
         <v>29</v>
       </c>
-      <c r="F9" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E10" t="s">
         <v>29</v>
       </c>
       <c r="F10" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>92</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -897,73 +903,73 @@
       <c r="E11" t="s">
         <v>29</v>
       </c>
+      <c r="F11" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>92</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>3</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" t="s">
         <v>29</v>
-      </c>
-      <c r="F12" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" t="s">
         <v>29</v>
       </c>
       <c r="F13" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" t="s">
         <v>29</v>
       </c>
       <c r="F14" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -975,32 +981,32 @@
         <v>29</v>
       </c>
       <c r="F15" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
         <v>71</v>
-      </c>
-      <c r="B16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <v>2</v>
-      </c>
-      <c r="E16" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="30">
-      <c r="A17" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="B17" t="s">
         <v>36</v>
@@ -1015,89 +1021,92 @@
         <v>29</v>
       </c>
       <c r="F17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="30">
+      <c r="A18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18">
-        <v>2</v>
-      </c>
-      <c r="E18" t="s">
-        <v>29</v>
-      </c>
-      <c r="F18" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="2" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="B19" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E19" t="s">
         <v>29</v>
       </c>
       <c r="F19" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="2" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="B20" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
       <c r="D20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20" t="s">
         <v>29</v>
       </c>
       <c r="F20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" t="s">
-        <v>75</v>
-      </c>
-      <c r="B21" t="s">
-        <v>65</v>
-      </c>
-      <c r="C21">
-        <v>-1</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="B22" t="s">
         <v>1</v>
@@ -1112,15 +1121,15 @@
         <v>30</v>
       </c>
       <c r="F22" t="s">
-        <v>59</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="C23">
         <v>-1</v>
@@ -1134,10 +1143,10 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C24">
         <v>-1</v>
@@ -1148,13 +1157,16 @@
       <c r="E24" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="F24" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="C25">
         <v>-1</v>
@@ -1165,56 +1177,50 @@
       <c r="E25" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F25" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>82</v>
+        <v>47</v>
       </c>
       <c r="B26" t="s">
-        <v>81</v>
+        <v>23</v>
       </c>
       <c r="C26">
         <v>-1</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="F26" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C27">
         <v>-1</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>30</v>
       </c>
       <c r="F27" t="s">
-        <v>88</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B28" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C28">
         <v>-1</v>
@@ -1224,14 +1230,17 @@
       </c>
       <c r="E28" s="1" t="s">
         <v>30</v>
+      </c>
+      <c r="F28" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="C29">
         <v>-1</v>
@@ -1243,15 +1252,15 @@
         <v>30</v>
       </c>
       <c r="F29" t="s">
-        <v>19</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>49</v>
+        <v>83</v>
       </c>
       <c r="B30" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="C30">
         <v>-1</v>
@@ -1261,14 +1270,11 @@
       </c>
       <c r="E30" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="F30" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B31" t="s">
         <v>45</v>
@@ -1282,13 +1288,16 @@
       <c r="E31" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="F31" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="B32" t="s">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="C32">
         <v>-1</v>
@@ -1298,14 +1307,17 @@
       </c>
       <c r="E32" s="1" t="s">
         <v>30</v>
+      </c>
+      <c r="F32" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B33" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="C33">
         <v>-1</v>
@@ -1319,7 +1331,7 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="B34" t="s">
         <v>1</v>
@@ -1332,17 +1344,14 @@
       </c>
       <c r="E34" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="F34" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B35" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C35">
         <v>-1</v>
@@ -1352,57 +1361,54 @@
       </c>
       <c r="E35" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="F35" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>70</v>
+        <v>31</v>
       </c>
       <c r="B36" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="C36">
         <v>-1</v>
       </c>
       <c r="D36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>30</v>
       </c>
       <c r="F36" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="B37" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="C37">
         <v>-1</v>
       </c>
       <c r="D37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>30</v>
       </c>
       <c r="F37" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>11</v>
+        <v>70</v>
       </c>
       <c r="B38" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C38">
         <v>-1</v>
@@ -1414,54 +1420,94 @@
         <v>30</v>
       </c>
       <c r="F38" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="B39" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="C39">
         <v>-1</v>
       </c>
       <c r="D39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="F39" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
+        <v>11</v>
+      </c>
+      <c r="B40" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40">
+        <v>-1</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F40" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41">
+        <v>-1</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F41" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
         <v>48</v>
       </c>
-      <c r="B40" t="s">
-        <v>1</v>
-      </c>
-      <c r="C40">
-        <v>-1</v>
-      </c>
-      <c r="D40">
-        <v>2</v>
-      </c>
-      <c r="E40" s="1" t="s">
+      <c r="B42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>-1</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F42" t="s">
         <v>67</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:F40">
-    <sortCondition descending="1" ref="C2:C40"/>
-    <sortCondition ref="E2:E40" customList="wip,todo,done"/>
-    <sortCondition ref="D2:D40"/>
+  <sortState ref="A2:F41">
+    <sortCondition descending="1" ref="C2:C41"/>
+    <sortCondition ref="E2:E41" customList="wip,todo,done"/>
+    <sortCondition ref="D2:D41"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
force explosive sur les bris de couverts
</commit_message>
<xml_diff>
--- a/TODO vertical slice.xlsx
+++ b/TODO vertical slice.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$F$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$F$35</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="101">
   <si>
     <t>Ajuster inclinaison du target viewer selon la pente de l'objet</t>
   </si>
@@ -321,13 +321,7 @@
     <t>Quand on lance une assiette sur un mur très proche, il ne faut pas qu'elle se casse (où quand deux assiettes sont déjà posées l'une sur l'autre sur le vaisselier par ex). Tout ça dépend de la surface de réception ? Utiliser le SciptableObject Surface prévu à cet effet.</t>
   </si>
   <si>
-    <t>Quand une assiette se casse sur un obstacle, il faut que les bris possèdent la même vélocité que l'assiette initiale (en particulier la même direction).</t>
-  </si>
-  <si>
-    <t>Débugger rendu 2D anims URP</t>
-  </si>
-  <si>
-    <t>Des sprites 2D qui s'affichent mal, suite au changement de rendu graphique en URP (Universal Render Pipeline)</t>
+    <t>Quand une assiette se casse sur un obstacle, il faut que les bris possèdent la même vélocité que l'assiette initiale (en particulier la même direction) =&gt; réglé plus simplement, en ajoutant une force explosive à chaque bris, ça fait le taf.</t>
   </si>
 </sst>
 </file>
@@ -693,10 +687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -731,10 +725,10 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>4</v>
@@ -746,15 +740,15 @@
         <v>51</v>
       </c>
       <c r="F2" t="s">
-        <v>102</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="C3">
         <v>4</v>
@@ -762,42 +756,42 @@
       <c r="D3">
         <v>2</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>51</v>
+      <c r="E3" t="s">
+        <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>100</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D4">
         <v>2</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>51</v>
+      <c r="E4" t="s">
+        <v>29</v>
       </c>
       <c r="F4" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -805,19 +799,16 @@
       <c r="E5" t="s">
         <v>29</v>
       </c>
-      <c r="F5" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -826,72 +817,72 @@
         <v>29</v>
       </c>
       <c r="F6" t="s">
-        <v>80</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>5</v>
       </c>
       <c r="C7">
         <v>3</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E7" t="s">
         <v>29</v>
       </c>
+      <c r="F7" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>91</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C8">
         <v>3</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E8" t="s">
         <v>29</v>
       </c>
-      <c r="F8" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" t="s">
         <v>29</v>
       </c>
       <c r="F9" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>91</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -902,13 +893,16 @@
       <c r="E10" t="s">
         <v>29</v>
       </c>
+      <c r="F10" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -920,78 +914,78 @@
         <v>29</v>
       </c>
       <c r="F11" t="s">
-        <v>62</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" t="s">
         <v>29</v>
       </c>
       <c r="F12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>98</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13" t="s">
         <v>29</v>
       </c>
-      <c r="F13" t="s">
-        <v>14</v>
+      <c r="F13" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14" t="s">
         <v>29</v>
       </c>
       <c r="F14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" t="s">
-        <v>98</v>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="30">
+      <c r="A15" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -999,19 +993,19 @@
       <c r="E15" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>99</v>
+      <c r="F15" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" t="s">
-        <v>71</v>
+      <c r="A16" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -1020,35 +1014,35 @@
         <v>29</v>
       </c>
       <c r="F16" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="30">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="2" t="s">
-        <v>37</v>
+        <v>76</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>77</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E17" t="s">
         <v>29</v>
       </c>
       <c r="F17" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="2" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>86</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1060,55 +1054,49 @@
         <v>29</v>
       </c>
       <c r="F18" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="2" t="s">
-        <v>76</v>
+      <c r="A19" t="s">
+        <v>64</v>
       </c>
       <c r="B19" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="C19">
+        <v>-1</v>
+      </c>
+      <c r="D19">
         <v>0</v>
       </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19" t="s">
-        <v>29</v>
-      </c>
-      <c r="F19" t="s">
-        <v>78</v>
+      <c r="E19" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="2" t="s">
-        <v>85</v>
+      <c r="A20" t="s">
+        <v>95</v>
       </c>
       <c r="B20" t="s">
-        <v>86</v>
+        <v>1</v>
       </c>
       <c r="C20">
+        <v>-1</v>
+      </c>
+      <c r="D20">
         <v>0</v>
       </c>
-      <c r="D20">
-        <v>2</v>
-      </c>
-      <c r="E20" t="s">
-        <v>29</v>
-      </c>
-      <c r="F20" t="s">
-        <v>87</v>
+      <c r="E20" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="C21">
         <v>-1</v>
@@ -1119,13 +1107,16 @@
       <c r="E21" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="F21" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="B22" t="s">
-        <v>1</v>
+        <v>65</v>
       </c>
       <c r="C22">
         <v>-1</v>
@@ -1139,7 +1130,7 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>89</v>
+        <v>58</v>
       </c>
       <c r="B23" t="s">
         <v>1</v>
@@ -1154,15 +1145,15 @@
         <v>30</v>
       </c>
       <c r="F23" t="s">
-        <v>90</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="C24">
         <v>-1</v>
@@ -1176,10 +1167,10 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B25" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C25">
         <v>-1</v>
@@ -1190,16 +1181,13 @@
       <c r="E25" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F25" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="C26">
         <v>-1</v>
@@ -1210,50 +1198,56 @@
       <c r="E26" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="F26" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>82</v>
       </c>
       <c r="B27" t="s">
-        <v>23</v>
+        <v>81</v>
       </c>
       <c r="C27">
         <v>-1</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>30</v>
+      </c>
+      <c r="F27" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C28">
         <v>-1</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>30</v>
       </c>
       <c r="F28" t="s">
-        <v>24</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B29" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C29">
         <v>-1</v>
@@ -1263,17 +1257,14 @@
       </c>
       <c r="E29" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="F29" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B30" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="C30">
         <v>-1</v>
@@ -1285,15 +1276,15 @@
         <v>30</v>
       </c>
       <c r="F30" t="s">
-        <v>88</v>
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="B31" t="s">
-        <v>84</v>
+        <v>50</v>
       </c>
       <c r="C31">
         <v>-1</v>
@@ -1303,11 +1294,14 @@
       </c>
       <c r="E31" s="1" t="s">
         <v>30</v>
+      </c>
+      <c r="F31" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B32" t="s">
         <v>45</v>
@@ -1321,16 +1315,13 @@
       <c r="E32" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F32" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="B33" t="s">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="C33">
         <v>-1</v>
@@ -1340,17 +1331,14 @@
       </c>
       <c r="E33" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="F33" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B34" t="s">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="C34">
         <v>-1</v>
@@ -1364,7 +1352,7 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="B35" t="s">
         <v>1</v>
@@ -1377,14 +1365,17 @@
       </c>
       <c r="E35" s="1" t="s">
         <v>30</v>
+      </c>
+      <c r="F35" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B36" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C36">
         <v>-1</v>
@@ -1394,11 +1385,14 @@
       </c>
       <c r="E36" s="1" t="s">
         <v>30</v>
+      </c>
+      <c r="F36" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="B37" t="s">
         <v>1</v>
@@ -1407,41 +1401,41 @@
         <v>-1</v>
       </c>
       <c r="D37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>30</v>
       </c>
       <c r="F37" t="s">
-        <v>32</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="B38" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="C38">
         <v>-1</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>30</v>
       </c>
       <c r="F38" t="s">
-        <v>35</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="B39" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="C39">
         <v>-1</v>
@@ -1453,15 +1447,15 @@
         <v>30</v>
       </c>
       <c r="F39" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="B40" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C40">
         <v>-1</v>
@@ -1473,15 +1467,15 @@
         <v>30</v>
       </c>
       <c r="F40" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="B41" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C41">
         <v>-1</v>
@@ -1493,66 +1487,46 @@
         <v>30</v>
       </c>
       <c r="F41" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="B42" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="C42">
         <v>-1</v>
       </c>
       <c r="D42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="F42" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="B43" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C43">
         <v>-1</v>
       </c>
       <c r="D43">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>55</v>
       </c>
       <c r="F43" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44" t="s">
-        <v>48</v>
-      </c>
-      <c r="B44" t="s">
-        <v>1</v>
-      </c>
-      <c r="C44">
-        <v>-1</v>
-      </c>
-      <c r="D44">
-        <v>2</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F44" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>